<commit_message>
3 new students was added
</commit_message>
<xml_diff>
--- a/BBI-23-1.xlsx
+++ b/BBI-23-1.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
   <si>
     <t>ФИО</t>
   </si>
@@ -253,6 +253,15 @@
   </si>
   <si>
     <t>ответ неверный в 1м номере</t>
+  </si>
+  <si>
+    <t>Алексеев Артем Алесандрович</t>
+  </si>
+  <si>
+    <t>Чайкина Софья Сергеевна</t>
+  </si>
+  <si>
+    <t>Ширшов Никита Сергеевич</t>
   </si>
 </sst>
 </file>
@@ -748,16 +757,16 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1676,10 +1685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T33"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,14 +1744,14 @@
       <c r="L1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="M1" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
       <c r="S1" s="18" t="s">
         <v>51</v>
       </c>
@@ -1789,12 +1798,12 @@
       <c r="L2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
       <c r="S2" s="11" t="s">
         <v>62</v>
       </c>
@@ -1839,12 +1848,12 @@
       <c r="L3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="46"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
       <c r="S3" s="11" t="s">
         <v>61</v>
       </c>
@@ -1889,12 +1898,12 @@
       <c r="L4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="47"/>
+      <c r="R4" s="47"/>
       <c r="S4" s="11" t="s">
         <v>52</v>
       </c>
@@ -1939,12 +1948,12 @@
       <c r="L5" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
       <c r="S5" s="11" t="s">
         <v>60</v>
       </c>
@@ -1987,12 +1996,12 @@
         <v>3</v>
       </c>
       <c r="L6" s="10"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="47"/>
+      <c r="R6" s="47"/>
       <c r="S6" s="11" t="s">
         <v>53</v>
       </c>
@@ -2035,12 +2044,12 @@
         <v>3</v>
       </c>
       <c r="L7" s="10"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="46"/>
-      <c r="P7" s="46"/>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="46"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="47"/>
       <c r="S7" s="11" t="s">
         <v>59</v>
       </c>
@@ -2083,12 +2092,12 @@
         <v>4</v>
       </c>
       <c r="L8" s="10"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="46"/>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="46"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="47"/>
+      <c r="R8" s="47"/>
       <c r="S8" s="11" t="s">
         <v>58</v>
       </c>
@@ -2133,12 +2142,12 @@
       <c r="L9" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="M9" s="46"/>
-      <c r="N9" s="46"/>
-      <c r="O9" s="46"/>
-      <c r="P9" s="46"/>
-      <c r="Q9" s="46"/>
-      <c r="R9" s="46"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="47"/>
+      <c r="R9" s="47"/>
       <c r="S9" s="11" t="s">
         <v>54</v>
       </c>
@@ -2183,14 +2192,14 @@
       <c r="L10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="M10" s="46" t="s">
+      <c r="M10" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="N10" s="46"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="46"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="47"/>
       <c r="S10" s="11" t="s">
         <v>57</v>
       </c>
@@ -2233,12 +2242,12 @@
         <v>2</v>
       </c>
       <c r="L11" s="10"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
       <c r="S11" s="11" t="s">
         <v>55</v>
       </c>
@@ -2283,12 +2292,12 @@
       <c r="L12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="46"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
       <c r="S12" s="11"/>
       <c r="T12" s="20"/>
     </row>
@@ -2331,12 +2340,12 @@
       <c r="L13" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="M13" s="46"/>
-      <c r="N13" s="46"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="46"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="47"/>
       <c r="S13" s="11" t="s">
         <v>71</v>
       </c>
@@ -2379,12 +2388,12 @@
         <v>3</v>
       </c>
       <c r="L14" s="10"/>
-      <c r="M14" s="46"/>
-      <c r="N14" s="46"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="46"/>
-      <c r="Q14" s="46"/>
-      <c r="R14" s="46"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
+      <c r="Q14" s="47"/>
+      <c r="R14" s="47"/>
       <c r="S14" s="11" t="s">
         <v>56</v>
       </c>
@@ -2429,12 +2438,12 @@
       <c r="L15" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="M15" s="46"/>
-      <c r="N15" s="46"/>
-      <c r="O15" s="46"/>
-      <c r="P15" s="46"/>
-      <c r="Q15" s="46"/>
-      <c r="R15" s="46"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="47"/>
       <c r="S15" s="11" t="s">
         <v>34</v>
       </c>
@@ -2477,12 +2486,12 @@
         <v>4</v>
       </c>
       <c r="L16" s="10"/>
-      <c r="M16" s="46"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="46"/>
-      <c r="P16" s="46"/>
-      <c r="Q16" s="46"/>
-      <c r="R16" s="46"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="47"/>
       <c r="S16" s="11" t="s">
         <v>64</v>
       </c>
@@ -2527,12 +2536,12 @@
       <c r="L17" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="46"/>
-      <c r="R17" s="46"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="47"/>
+      <c r="R17" s="47"/>
       <c r="S17" s="11" t="s">
         <v>63</v>
       </c>
@@ -2577,12 +2586,12 @@
       <c r="L18" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="M18" s="46"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="46"/>
-      <c r="Q18" s="46"/>
-      <c r="R18" s="46"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="47"/>
+      <c r="O18" s="47"/>
+      <c r="P18" s="47"/>
+      <c r="Q18" s="47"/>
+      <c r="R18" s="47"/>
       <c r="S18" s="11" t="s">
         <v>65</v>
       </c>
@@ -2627,12 +2636,12 @@
       <c r="L19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="46"/>
-      <c r="Q19" s="46"/>
-      <c r="R19" s="46"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="47"/>
+      <c r="P19" s="47"/>
+      <c r="Q19" s="47"/>
+      <c r="R19" s="47"/>
       <c r="S19" s="11" t="s">
         <v>34</v>
       </c>
@@ -2679,14 +2688,14 @@
       <c r="L20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="M20" s="46" t="s">
+      <c r="M20" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="N20" s="46"/>
-      <c r="O20" s="46"/>
-      <c r="P20" s="46"/>
-      <c r="Q20" s="46"/>
-      <c r="R20" s="46"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="47"/>
+      <c r="P20" s="47"/>
+      <c r="Q20" s="47"/>
+      <c r="R20" s="47"/>
       <c r="S20" s="11" t="s">
         <v>66</v>
       </c>
@@ -2731,12 +2740,12 @@
       <c r="L21" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="M21" s="46"/>
-      <c r="N21" s="46"/>
-      <c r="O21" s="46"/>
-      <c r="P21" s="46"/>
-      <c r="Q21" s="46"/>
-      <c r="R21" s="46"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="47"/>
+      <c r="R21" s="47"/>
       <c r="S21" s="11" t="s">
         <v>67</v>
       </c>
@@ -2781,14 +2790,14 @@
       <c r="L22" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="M22" s="46" t="s">
+      <c r="M22" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="N22" s="46"/>
-      <c r="O22" s="46"/>
-      <c r="P22" s="46"/>
-      <c r="Q22" s="46"/>
-      <c r="R22" s="46"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="47"/>
+      <c r="Q22" s="47"/>
+      <c r="R22" s="47"/>
       <c r="S22" s="11" t="s">
         <v>68</v>
       </c>
@@ -2833,14 +2842,14 @@
       <c r="L23" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="M23" s="46" t="s">
+      <c r="M23" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="N23" s="46"/>
-      <c r="O23" s="46"/>
-      <c r="P23" s="46"/>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="46"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="47"/>
+      <c r="P23" s="47"/>
+      <c r="Q23" s="47"/>
+      <c r="R23" s="47"/>
       <c r="S23" s="11" t="s">
         <v>69</v>
       </c>
@@ -2883,12 +2892,12 @@
         <v>4</v>
       </c>
       <c r="L24" s="10"/>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="46"/>
-      <c r="P24" s="46"/>
-      <c r="Q24" s="46"/>
-      <c r="R24" s="46"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="47"/>
+      <c r="P24" s="47"/>
+      <c r="Q24" s="47"/>
+      <c r="R24" s="47"/>
       <c r="S24" s="11" t="s">
         <v>70</v>
       </c>
@@ -2933,19 +2942,19 @@
       <c r="L25" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="M25" s="49"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="49"/>
-      <c r="P25" s="49"/>
-      <c r="Q25" s="49"/>
-      <c r="R25" s="49"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="48"/>
+      <c r="O25" s="48"/>
+      <c r="P25" s="48"/>
+      <c r="Q25" s="48"/>
+      <c r="R25" s="48"/>
       <c r="S25" s="15" t="s">
         <v>34</v>
       </c>
       <c r="T25" s="21"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="46" t="s">
         <v>72</v>
       </c>
       <c r="B27" s="26"/>
@@ -2954,7 +2963,7 @@
       <c r="E27" s="26"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
+      <c r="A28" s="46"/>
       <c r="B28" s="27">
         <v>2</v>
       </c>
@@ -2969,7 +2978,7 @@
       </c>
     </row>
     <row r="29" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="46" t="s">
         <v>73</v>
       </c>
       <c r="B29" s="35"/>
@@ -2978,14 +2987,14 @@
       <c r="E29" s="35"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="48"/>
+      <c r="A30" s="46"/>
       <c r="B30" s="35"/>
       <c r="C30" s="35"/>
       <c r="D30" s="35"/>
       <c r="E30" s="35"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="36">
         <v>2</v>
       </c>
@@ -2996,23 +3005,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
       <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="M18:R18"/>
-    <mergeCell ref="M16:R16"/>
-    <mergeCell ref="M17:R17"/>
-    <mergeCell ref="M20:R20"/>
-    <mergeCell ref="M25:R25"/>
-    <mergeCell ref="M19:R19"/>
-    <mergeCell ref="M21:R21"/>
-    <mergeCell ref="M22:R22"/>
-    <mergeCell ref="M23:R23"/>
-    <mergeCell ref="M24:R24"/>
     <mergeCell ref="M7:R7"/>
     <mergeCell ref="M8:R8"/>
     <mergeCell ref="M9:R9"/>
@@ -3028,6 +3038,18 @@
     <mergeCell ref="M12:R12"/>
     <mergeCell ref="M13:R13"/>
     <mergeCell ref="M14:R14"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="M18:R18"/>
+    <mergeCell ref="M16:R16"/>
+    <mergeCell ref="M17:R17"/>
+    <mergeCell ref="M20:R20"/>
+    <mergeCell ref="M25:R25"/>
+    <mergeCell ref="M19:R19"/>
+    <mergeCell ref="M21:R21"/>
+    <mergeCell ref="M22:R22"/>
+    <mergeCell ref="M23:R23"/>
+    <mergeCell ref="M24:R24"/>
   </mergeCells>
   <conditionalFormatting sqref="L2:L3 L6:L8 L19 L16 L14 L24:L25 L10:L12">
     <cfRule type="cellIs" dxfId="62" priority="101" operator="equal">

</xml_diff>